<commit_message>
use daily factor data only and correct VIX hedge return
</commit_message>
<xml_diff>
--- a/factor_regime_analysis.xlsx
+++ b/factor_regime_analysis.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,161 +465,81 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DAILY</t>
+          <t>Growth</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0596634612499026</v>
+        <v>4.224307243328472</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01559896120181423</v>
+        <v>-1.389314965282897</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01990802406500616</v>
+        <v>-0.4992333201825374</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factor_4</t>
+          <t>Momentum</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2327530769748014</v>
+        <v>23.27530769748014</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003923735345141588</v>
+        <v>0.3923735345141589</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.04524771399983118</v>
+        <v>-4.524771399983118</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factor_7</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.1660885658902768</v>
+        <v>-16.60885658902768</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01986984739307428</v>
+        <v>1.986984739307428</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.01146493963035807</v>
+        <v>-1.146493963035807</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factor_10</t>
+          <t>Qualiy</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.05777747455722276</v>
+        <v>5.777747455722276</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01078942965778431</v>
+        <v>1.078942965778432</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.02160583007445909</v>
+        <v>-2.160583007445909</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factor_13</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.09763055541979587</v>
+        <v>9.763055541979588</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03283780503056711</v>
+        <v>3.283780503056711</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001125963018485632</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WEEKLY</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.04224307243328471</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-0.01389314965282897</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.004992333201825374</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Factor_20</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.1729437001781768</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0756745284219212</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-0.08724585569551024</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Factor_23</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.09285872768620682</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-0.03870019490935461</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.002178962745435704</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Factor_26</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.02582593079148412</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.05026981501458693</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.04506032846615894</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Factor_29</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0.06492261584723666</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.06241722155734662</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-0.007954355658339759</v>
+        <v>0.1125963018485632</v>
       </c>
     </row>
   </sheetData>
@@ -633,7 +553,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -706,47 +626,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DAILY</t>
+          <t>Growth</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>685</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0002367597668646929</v>
+        <v>0.0001676312398146219</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003327036328042688</v>
+        <v>0.003116708205195317</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0596634612499026</v>
+        <v>0.04224307243328471</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05281506436127078</v>
+        <v>0.04947620892060767</v>
       </c>
       <c r="G2" t="n">
-        <v>1.129667491111755</v>
+        <v>0.8538057655361257</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5182481751824818</v>
+        <v>0.1153284671532847</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.01185700276366231</v>
+        <v>-0.02321510824504835</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0131091479053862</v>
+        <v>0.02161698885820384</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0001871782873188454</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1668860165302586</v>
+        <v>0.4764312813188127</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factor_4</t>
+          <t>Momentum</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -786,7 +706,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factor_7</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -826,7 +746,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factor_10</t>
+          <t>Qualiy</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -866,7 +786,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factor_13</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -901,206 +821,6 @@
       </c>
       <c r="L6" t="n">
         <v>-1.310814479956729</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WEEKLY</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>685</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0001676312398146219</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.003116708205195317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.04224307243328471</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.04947620892060767</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.8538057655361257</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.1153284671532847</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-0.02321510824504835</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.02161698885820384</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.4764312813188127</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Factor_20</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>685</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0006862845245165746</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.008064342499274129</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.1729437001781768</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1280174684419706</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1.350938292117306</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.1153284671532847</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-0.05040595399188108</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.06489950843133574</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1.411283329660923</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Factor_23</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>685</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-0.0003684870146278048</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.00622615596493388</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-0.09285872768620682</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.09883716184269861</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-0.9395122841952241</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.07445255474452554</v>
-      </c>
-      <c r="I9" t="n">
-        <v>-0.04281488401058708</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.04070796460176984</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>-0.5761016330160517</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Factor_26</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>685</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.0001024838523471592</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.004608572859132715</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.02582593079148412</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.07315882610512242</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.3530118260013449</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.1065693430656934</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-0.02540154248920967</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.03249384860327087</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.318924760660549</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Factor_29</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>685</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.0002576294279652248</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.006339664663537337</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.06492261584723666</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.1006390565715826</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.6451035816403791</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.1021897810218978</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-0.04351572598018094</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.07634438562273616</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>2.532984880252076</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +834,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1187,47 +907,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DAILY</t>
+          <t>Growth</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>986</v>
       </c>
       <c r="C2" t="n">
-        <v>-6.190063968973899e-05</v>
+        <v>-5.51315462413848e-05</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003301860735154769</v>
+        <v>0.003130133596255772</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.01559896120181423</v>
+        <v>-0.01389314965282897</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05241541421393054</v>
+        <v>0.04968933039660618</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.2976025551977506</v>
+        <v>-0.2796002590885766</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4756592292089249</v>
+        <v>0.103448275862069</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.01327729487057028</v>
+        <v>-0.02481592582492509</v>
       </c>
       <c r="J2" t="n">
-        <v>0.01291896286927452</v>
+        <v>0.01613795647362593</v>
       </c>
       <c r="K2" t="n">
-        <v>-9.357844098417667e-05</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.1052878709471754</v>
+        <v>-1.178007239640821</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factor_4</t>
+          <t>Momentum</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1267,7 +987,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factor_7</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1307,7 +1027,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factor_10</t>
+          <t>Qualiy</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1347,7 +1067,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factor_13</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1382,206 +1102,6 @@
       </c>
       <c r="L6" t="n">
         <v>-0.09856115618522132</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WEEKLY</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>986</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-5.51315462413848e-05</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.003130133596255772</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-0.01389314965282897</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.04968933039660618</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-0.2796002590885766</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.103448275862069</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-0.02481592582492509</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.01613795647362593</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>-1.178007239640821</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Factor_20</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>986</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0003002957477060365</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.01050242925881057</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.0756745284219212</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1667208958851672</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.453899482846132</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.1135902636916836</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-0.1141024784554745</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.05387390213299859</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-2.48284907448052</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Factor_23</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>986</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-0.0001535722020212485</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.005710295377304341</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-0.03870019490935461</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.0906481288864142</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-0.4269276750085767</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.09229208924949291</v>
-      </c>
-      <c r="I9" t="n">
-        <v>-0.04447170679343648</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.07491262726029468</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>2.275330501575194</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Factor_26</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>986</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.0001994833929150275</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.004497890798250356</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.05026981501458693</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.07140180285897742</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.7040412566874907</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.1075050709939148</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-0.03137553677794713</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.02949965519883557</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.8547516320789778</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Factor_29</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>986</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.0002476873871323278</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.005164648071008975</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.06241722155734662</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.08198624643035522</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.761313321135736</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.116632860040568</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-0.02907220822837953</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.03402625820568916</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.7951956910124707</v>
       </c>
     </row>
   </sheetData>
@@ -1595,7 +1115,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1668,47 +1188,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DAILY</t>
+          <t>Growth</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C2" t="n">
-        <v>-7.900009549605621e-05</v>
+        <v>-1.981084603898958e-05</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003091535078367284</v>
+        <v>0.003025665016521365</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.01990802406500616</v>
+        <v>-0.004992333201825374</v>
       </c>
       <c r="F2" t="n">
-        <v>0.04907659792075448</v>
+        <v>0.048030943105822</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.4056520807972931</v>
+        <v>-0.1039399370282245</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4934210526315789</v>
+        <v>0.1015831134564644</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.01527938171804211</v>
+        <v>-0.02283063489175907</v>
       </c>
       <c r="J2" t="n">
-        <v>0.01013312139876832</v>
+        <v>0.01492248062015489</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.3351277304306014</v>
+        <v>-1.473431113302525</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factor_4</t>
+          <t>Momentum</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1748,7 +1268,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factor_7</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1788,7 +1308,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factor_10</t>
+          <t>Qualiy</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1828,7 +1348,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factor_13</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1863,206 +1383,6 @@
       </c>
       <c r="L6" t="n">
         <v>-0.5831737516658294</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WEEKLY</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>758</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-1.981084603898958e-05</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.003025665016521365</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-0.004992333201825374</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.048030943105822</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-0.1039399370282245</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.1015831134564644</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-0.02283063489175907</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.01492248062015489</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>-1.473431113302525</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Factor_20</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>758</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-0.0003462137130774216</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.008884382505405792</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-0.08724585569551024</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1410351999700601</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-0.6186105008822718</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.09102902374670185</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-0.09713342957310778</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.05421785421785419</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-1.812888928370654</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Factor_23</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>758</v>
-      </c>
-      <c r="C9" t="n">
-        <v>8.646677561252796e-06</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.005957980559985805</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.002178962745435704</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.09458000926727873</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.02303830124691632</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.1002638522427441</v>
-      </c>
-      <c r="I9" t="n">
-        <v>-0.0490906604676602</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.03827591945415199</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>-0.6358524512558048</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Factor_26</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>758</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-0.0001788108272466625</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.00426516845054771</v>
-      </c>
-      <c r="E10" t="n">
-        <v>-0.04506032846615894</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.0677074501196876</v>
-      </c>
-      <c r="G10" t="n">
-        <v>-0.6655150708896148</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.1002638522427441</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-0.02733016256122667</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.02356043956043963</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>-1.043704987661976</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Factor_29</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>758</v>
-      </c>
-      <c r="C11" t="n">
-        <v>-3.156490340611016e-05</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.004702121460798033</v>
-      </c>
-      <c r="E11" t="n">
-        <v>-0.007954355658339759</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.07464386411814806</v>
-      </c>
-      <c r="G11" t="n">
-        <v>-0.1065640927397518</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.09894459102902374</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-0.03104634322954392</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.02379132428817132</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>-1.153758506453692</v>
       </c>
     </row>
   </sheetData>
@@ -2076,7 +1396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2109,7 +1429,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Factor_7</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -2127,14 +1447,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factor_23</t>
+          <t>Growth</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.03099238538522137</v>
+        <v>-0.006239015397916688</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1267518727655036</v>
+        <v>0.7585892515235535</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -2145,14 +1465,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>WEEKLY</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.006239015397916688</v>
+        <v>-0.0155625745099148</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7585892515235535</v>
+        <v>0.4431010065015112</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -2163,14 +1483,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factor_13</t>
+          <t>Qualiy</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.0155625745099148</v>
+        <v>-0.03438862748039828</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4431010065015112</v>
+        <v>0.09004383673953691</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -2181,106 +1501,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factor_26</t>
+          <t>Momentum</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.02870950205377392</v>
+        <v>-0.05644788198630889</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1572128684773395</v>
+        <v>0.005369950154660545</v>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Factor_29</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>-0.03105371580178276</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.1260018678377664</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>DAILY</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>-0.03319947695431829</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.1017318180015465</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Factor_10</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.03438862748039828</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.09004383673953691</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Factor_20</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>-0.05046399640768519</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.01286744882654438</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Factor_4</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>-0.05644788198630889</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.005369950154660545</v>
-      </c>
-      <c r="D11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -2297,7 +1527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2330,23 +1560,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DAILY</t>
+          <t>Growth</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.129667491111755</v>
+        <v>0.8538057655361257</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2976025551977506</v>
+        <v>-0.2796002590885766</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.4056520807972931</v>
+        <v>-0.1039399370282245</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factor_4</t>
+          <t>Momentum</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2362,7 +1592,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factor_7</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2378,7 +1608,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factor_10</t>
+          <t>Qualiy</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2394,7 +1624,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factor_13</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2405,86 +1635,6 @@
       </c>
       <c r="D6" t="n">
         <v>0.01405615396030617</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WEEKLY</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.8538057655361257</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-0.2796002590885766</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.1039399370282245</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Factor_20</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1.350938292117306</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.453899482846132</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-0.6186105008822718</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Factor_23</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.9395122841952241</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-0.4269276750085767</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.02303830124691632</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Factor_26</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.3530118260013449</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.7040412566874907</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.6655150708896148</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Factor_29</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0.6451035816403791</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.761313321135736</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-0.1065640927397518</v>
       </c>
     </row>
   </sheetData>
@@ -2498,7 +1648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2531,23 +1681,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DAILY</t>
+          <t>Growth</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51.82481751824818</v>
+        <v>11.53284671532847</v>
       </c>
       <c r="C2" t="n">
-        <v>47.5659229208925</v>
+        <v>10.3448275862069</v>
       </c>
       <c r="D2" t="n">
-        <v>49.34210526315789</v>
+        <v>10.15831134564644</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factor_4</t>
+          <t>Momentum</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2563,7 +1713,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factor_7</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2579,7 +1729,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factor_10</t>
+          <t>Qualiy</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2595,7 +1745,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factor_13</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2606,86 +1756,6 @@
       </c>
       <c r="D6" t="n">
         <v>52.5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WEEKLY</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>11.53284671532847</v>
-      </c>
-      <c r="C7" t="n">
-        <v>10.3448275862069</v>
-      </c>
-      <c r="D7" t="n">
-        <v>10.15831134564644</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Factor_20</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>11.53284671532847</v>
-      </c>
-      <c r="C8" t="n">
-        <v>11.35902636916836</v>
-      </c>
-      <c r="D8" t="n">
-        <v>9.102902374670185</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Factor_23</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>7.445255474452554</v>
-      </c>
-      <c r="C9" t="n">
-        <v>9.22920892494929</v>
-      </c>
-      <c r="D9" t="n">
-        <v>10.02638522427441</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Factor_26</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>10.65693430656934</v>
-      </c>
-      <c r="C10" t="n">
-        <v>10.75050709939148</v>
-      </c>
-      <c r="D10" t="n">
-        <v>10.02638522427441</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Factor_29</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>10.21897810218978</v>
-      </c>
-      <c r="C11" t="n">
-        <v>11.6632860040568</v>
-      </c>
-      <c r="D11" t="n">
-        <v>9.894459102902374</v>
       </c>
     </row>
   </sheetData>
@@ -2699,7 +1769,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2732,23 +1802,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DAILY</t>
+          <t>Growth</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.281506436127078</v>
+        <v>4.947620892060767</v>
       </c>
       <c r="C2" t="n">
-        <v>5.241541421393054</v>
+        <v>4.968933039660619</v>
       </c>
       <c r="D2" t="n">
-        <v>4.907659792075448</v>
+        <v>4.803094310582201</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factor_4</t>
+          <t>Momentum</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2764,7 +1834,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factor_7</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2780,7 +1850,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factor_10</t>
+          <t>Qualiy</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2796,7 +1866,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factor_13</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2807,86 +1877,6 @@
       </c>
       <c r="D6" t="n">
         <v>8.010463044622956</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WEEKLY</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>4.947620892060767</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4.968933039660619</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4.803094310582201</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Factor_20</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>12.80174684419706</v>
-      </c>
-      <c r="C8" t="n">
-        <v>16.67208958851672</v>
-      </c>
-      <c r="D8" t="n">
-        <v>14.10351999700601</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Factor_23</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>9.883716184269861</v>
-      </c>
-      <c r="C9" t="n">
-        <v>9.06481288864142</v>
-      </c>
-      <c r="D9" t="n">
-        <v>9.458000926727873</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Factor_26</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>7.315882610512242</v>
-      </c>
-      <c r="C10" t="n">
-        <v>7.140180285897742</v>
-      </c>
-      <c r="D10" t="n">
-        <v>6.77074501196876</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Factor_29</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>10.06390565715826</v>
-      </c>
-      <c r="C11" t="n">
-        <v>8.198624643035522</v>
-      </c>
-      <c r="D11" t="n">
-        <v>7.464386411814806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>